<commit_message>
updated documentation and codes
</commit_message>
<xml_diff>
--- a/grafy.xlsx
+++ b/grafy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eltody\Documents\GitHub\VUT_FIT_IMS_proj1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F100F02D-7DF4-48E8-B4DA-EC69848CCC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502FFCDF-3C66-4798-90D0-EDDE2DC6B534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{3EE7ABC8-E057-4999-983D-E0D4547F23DB}"/>
   </bookViews>
@@ -34,18 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>else</t>
+    <t>number of electric cars</t>
   </si>
   <si>
-    <t>electric cars consumption</t>
+    <t>real number of ev</t>
   </si>
   <si>
-    <t>number of electric cars</t>
+    <t>global energy consumption</t>
+  </si>
+  <si>
+    <t>electric cars energy consumption</t>
   </si>
 </sst>
 </file>
@@ -115,75 +118,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="sk-SK"/>
-              <a:t>World</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="sk-SK" baseline="0"/>
-              <a:t> e</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="sk-SK"/>
-              <a:t>lectricity</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="sk-SK" baseline="0"/>
-              <a:t> consumption</a:t>
-            </a:r>
-            <a:endParaRPr lang="sk-SK"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:view3D>
       <c:rotX val="15"/>
       <c:rotY val="20"/>
@@ -238,7 +173,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>electric cars consumption</c:v>
+                  <c:v>electric cars energy consumption</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -333,67 +268,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>13.3514</c:v>
+                  <c:v>13.886200000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.078900000000001</c:v>
+                  <c:v>19.839200000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.2529</c:v>
+                  <c:v>28.340499999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.932200000000002</c:v>
+                  <c:v>40.4876</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.611199999999997</c:v>
+                  <c:v>57.829599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.454599999999999</c:v>
+                  <c:v>82.642099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.51</c:v>
+                  <c:v>118.044</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>162.15199999999999</c:v>
+                  <c:v>168.624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>231.64699999999999</c:v>
+                  <c:v>240.90199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>330.93599999999998</c:v>
+                  <c:v>344.15699999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>472.77600000000001</c:v>
+                  <c:v>491.66699999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>675.38199999999995</c:v>
+                  <c:v>702.36699999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>964.85299999999995</c:v>
+                  <c:v>1003.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1378.36</c:v>
+                  <c:v>1433.41</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1969.1</c:v>
+                  <c:v>2047.78</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2813.03</c:v>
+                  <c:v>2925.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4018.64</c:v>
+                  <c:v>4179.16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5740.93</c:v>
+                  <c:v>5970.28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8201.39</c:v>
+                  <c:v>8529.02</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11716.3</c:v>
+                  <c:v>12184.4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16737.8</c:v>
+                  <c:v>17406.400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -413,7 +348,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>else</c:v>
+                  <c:v>global energy consumption</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -511,49 +446,64 @@
                   <c:v>23398</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24300</c:v>
+                  <c:v>24100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25200</c:v>
+                  <c:v>24800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26200</c:v>
+                  <c:v>25600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27250</c:v>
+                  <c:v>26350</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28500</c:v>
+                  <c:v>27150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29700</c:v>
+                  <c:v>27990</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31100</c:v>
+                  <c:v>29000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32700</c:v>
+                  <c:v>30100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34300</c:v>
+                  <c:v>31300</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36100</c:v>
+                  <c:v>32400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38100</c:v>
+                  <c:v>33550</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40100</c:v>
+                  <c:v>34700</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42300</c:v>
+                  <c:v>35900</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44300</c:v>
+                  <c:v>37400</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46400</c:v>
+                  <c:v>38600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -870,7 +820,1140 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sk-SK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>Electric</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" baseline="0"/>
+              <a:t> cars in the world</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sk-SK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Real data</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hárok1!$C$28:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hárok1!$D$28:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5200000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10300000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FEB0-4D46-9D17-0C81A90724C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Model data</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hárok1!$C$28:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hárok1!$E$28:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5200000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7430312</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10612498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FEB0-4D46-9D17-0C81A90724C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1653066448"/>
+        <c:axId val="1653065200"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hárok1!$C$28:$C$30</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hárok1!$C$28:$C$30</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-FEB0-4D46-9D17-0C81A90724C8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1653066448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sk-SK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1653065200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1653065200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Number of electric</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="sk-SK" baseline="0"/>
+                  <a:t> cars</a:t>
+                </a:r>
+                <a:endParaRPr lang="sk-SK"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sk-SK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1653066448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sk-SK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sk-SK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sk-SK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sk-SK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hárok1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>number of electric cars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hárok1!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2038</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hárok1!$F$4:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>5200000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7430312</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10612498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15161152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21655966</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30942797</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44207472</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63151078</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90215959</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128881843</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>184118036</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>263031045</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>375756633</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>536799110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>766859592</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1095522875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1565043898</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2235790055</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3194012619</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4562898225</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6518478523</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4D52-4795-9540-94485E46666A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1590623520"/>
+        <c:axId val="1590628512"/>
+        <c:axId val="1795910240"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1590623520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1590628512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1590628512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1590623520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="1795910240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1590628512"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sk-SK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1404,20 +2487,1030 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:colOff>432995</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:rowOff>30704</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>280595</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>42134</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1437,6 +3530,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390608</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>29818</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1258625</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>175592</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graf 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E72BF5-C807-47F6-9CB5-B5D52A24694B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graf 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3272731E-2EB8-45E3-AEEE-727B3CB08826}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1742,213 +3907,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BB0E1F-EFBD-4BD9-A420-FAC1503FCD2E}">
-  <dimension ref="C3:F24"/>
+  <dimension ref="C3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
     <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
     <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
+      <c r="H3" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2018</v>
       </c>
       <c r="D4">
-        <v>13.3514</v>
+        <v>13.886200000000001</v>
       </c>
       <c r="E4">
         <v>23398</v>
       </c>
       <c r="F4">
-        <v>5000000</v>
+        <v>5200000</v>
+      </c>
+      <c r="G4">
+        <v>5200000</v>
+      </c>
+      <c r="H4">
+        <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2019</v>
       </c>
       <c r="D5">
-        <v>19.078900000000001</v>
+        <v>19.839200000000002</v>
       </c>
       <c r="E5">
-        <v>24300</v>
+        <v>24100</v>
       </c>
       <c r="F5">
-        <v>7144923</v>
+        <v>7430312</v>
+      </c>
+      <c r="G5">
+        <v>7100000</v>
+      </c>
+      <c r="H5">
+        <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>2020</v>
       </c>
       <c r="D6">
-        <v>27.2529</v>
+        <v>28.340499999999999</v>
       </c>
       <c r="E6">
-        <v>25200</v>
+        <v>24800</v>
       </c>
       <c r="F6">
-        <v>10204815</v>
+        <v>10612498</v>
+      </c>
+      <c r="G6">
+        <v>10200000</v>
+      </c>
+      <c r="H6">
+        <v>2020</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>2021</v>
       </c>
       <c r="D7">
-        <v>38.932200000000002</v>
+        <v>40.4876</v>
       </c>
       <c r="E7">
-        <v>26200</v>
+        <v>25600</v>
       </c>
       <c r="F7">
-        <v>14578966</v>
+        <v>15161152</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>2022</v>
       </c>
       <c r="D8">
-        <v>55.611199999999997</v>
+        <v>57.829599999999999</v>
       </c>
       <c r="E8">
-        <v>27250</v>
+        <v>26350</v>
       </c>
       <c r="F8">
-        <v>20823689</v>
+        <v>21655966</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>2023</v>
       </c>
       <c r="D9">
-        <v>79.454599999999999</v>
+        <v>82.642099999999999</v>
       </c>
       <c r="E9">
-        <v>28500</v>
+        <v>27150</v>
       </c>
       <c r="F9">
-        <v>29752268</v>
+        <v>30942797</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>2024</v>
       </c>
       <c r="D10">
-        <v>113.51</v>
+        <v>118.044</v>
       </c>
       <c r="E10">
-        <v>29700</v>
+        <v>27990</v>
       </c>
       <c r="F10">
-        <v>42508940</v>
+        <v>44207472</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>2025</v>
       </c>
       <c r="D11">
-        <v>162.15199999999999</v>
+        <v>168.624</v>
       </c>
       <c r="E11">
-        <v>31100</v>
+        <v>29000</v>
       </c>
       <c r="F11">
-        <v>60724583</v>
+        <v>63151078</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>2026</v>
       </c>
       <c r="D12">
-        <v>231.64699999999999</v>
+        <v>240.90199999999999</v>
       </c>
       <c r="E12">
-        <v>32700</v>
+        <v>30100</v>
       </c>
       <c r="F12">
-        <v>86750483</v>
+        <v>90215959</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>2027</v>
       </c>
       <c r="D13">
-        <v>330.93599999999998</v>
+        <v>344.15699999999998</v>
       </c>
       <c r="E13">
-        <v>34300</v>
+        <v>31300</v>
       </c>
       <c r="F13">
-        <v>123928155</v>
+        <v>128881843</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>2028</v>
       </c>
       <c r="D14">
-        <v>472.77600000000001</v>
+        <v>491.66699999999997</v>
       </c>
       <c r="E14">
-        <v>36100</v>
+        <v>32400</v>
       </c>
       <c r="F14">
-        <v>177048493</v>
+        <v>184118036</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>2029</v>
       </c>
       <c r="D15">
-        <v>675.38199999999995</v>
+        <v>702.36699999999996</v>
       </c>
       <c r="E15">
-        <v>38100</v>
+        <v>33550</v>
       </c>
       <c r="F15">
-        <v>252921655</v>
+        <v>263031045</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>2030</v>
       </c>
       <c r="D16">
-        <v>964.85299999999995</v>
+        <v>1003.4</v>
       </c>
       <c r="E16">
-        <v>40100</v>
+        <v>34700</v>
       </c>
       <c r="F16">
-        <v>361324738</v>
+        <v>375756633</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
@@ -1956,13 +4147,13 @@
         <v>2031</v>
       </c>
       <c r="D17">
-        <v>1378.36</v>
+        <v>1433.41</v>
       </c>
       <c r="E17">
-        <v>42300</v>
+        <v>35900</v>
       </c>
       <c r="F17">
-        <v>516179704</v>
+        <v>536799110</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">
@@ -1970,13 +4161,13 @@
         <v>2032</v>
       </c>
       <c r="D18">
-        <v>1969.1</v>
+        <v>2047.78</v>
       </c>
       <c r="E18">
-        <v>44300</v>
+        <v>37400</v>
       </c>
       <c r="F18">
-        <v>737405587</v>
+        <v>766859592</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
@@ -1984,13 +4175,13 @@
         <v>2033</v>
       </c>
       <c r="D19">
-        <v>2813.03</v>
+        <v>2925.4</v>
       </c>
       <c r="E19">
-        <v>46400</v>
+        <v>38600</v>
       </c>
       <c r="F19">
-        <v>1053437901</v>
+        <v>1095522875</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.3">
@@ -1998,10 +4189,13 @@
         <v>2034</v>
       </c>
       <c r="D20">
-        <v>4018.64</v>
+        <v>4179.16</v>
+      </c>
+      <c r="E20">
+        <v>40000</v>
       </c>
       <c r="F20">
-        <v>1504926559</v>
+        <v>1565043898</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.3">
@@ -2009,10 +4203,13 @@
         <v>2035</v>
       </c>
       <c r="D21">
-        <v>5740.93</v>
+        <v>5970.28</v>
+      </c>
+      <c r="E21">
+        <v>41300</v>
       </c>
       <c r="F21">
-        <v>2149907090</v>
+        <v>2235790055</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
@@ -2020,10 +4217,13 @@
         <v>2036</v>
       </c>
       <c r="D22">
-        <v>8201.39</v>
+        <v>8529.02</v>
+      </c>
+      <c r="E22">
+        <v>42200</v>
       </c>
       <c r="F22">
-        <v>3071314653</v>
+        <v>3194012619</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
@@ -2031,10 +4231,13 @@
         <v>2037</v>
       </c>
       <c r="D23">
-        <v>11716.3</v>
+        <v>12184.4</v>
+      </c>
+      <c r="E23">
+        <v>43500</v>
       </c>
       <c r="F23">
-        <v>4387620466</v>
+        <v>4562898225</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.3">
@@ -2042,10 +4245,57 @@
         <v>2038</v>
       </c>
       <c r="D24">
-        <v>16737.8</v>
+        <v>17406.400000000001</v>
+      </c>
+      <c r="E24">
+        <v>44900</v>
       </c>
       <c r="F24">
-        <v>6268069171</v>
+        <v>6518478523</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>2018</v>
+      </c>
+      <c r="D28">
+        <v>5200000</v>
+      </c>
+      <c r="E28">
+        <v>5200000</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>2019</v>
+      </c>
+      <c r="D29">
+        <v>7200000</v>
+      </c>
+      <c r="E29">
+        <v>7430312</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>2020</v>
+      </c>
+      <c r="D30">
+        <v>10300000</v>
+      </c>
+      <c r="E30">
+        <v>10612498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>